<commit_message>
add file bab 4 & fix revisi
</commit_message>
<xml_diff>
--- a/DOKUMENT/kuesioner masya.xlsx
+++ b/DOKUMENT/kuesioner masya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SKRIPSI\DOKUMENT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAD9AF1-7F5C-46C1-84F1-4D8F62461E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FADF524-AF3A-4F3E-AEE5-FBA8DA63CC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="188">
   <si>
     <t>Timestamp</t>
   </si>
@@ -419,6 +419,183 @@
   </si>
   <si>
     <t>Kesimpulan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,80 &lt; 𝑟11 ≤ 1,00 </t>
+  </si>
+  <si>
+    <t>Reliabilitas sangat tinggi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,60 &lt; 𝑟11 ≤ 0,80 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reliabilitas tinggi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,40 &lt; 𝑟11 ≤ 0,60 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reliabilitas sedang </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,20 &lt; 𝑟11 ≤ 0,40 </t>
+  </si>
+  <si>
+    <t>Reliabilitas rendah</t>
+  </si>
+  <si>
+    <t>Tidak reliable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,00 &lt; 𝑟11 ≤ 0,20 </t>
+  </si>
+  <si>
+    <t>Usability</t>
+  </si>
+  <si>
+    <t>Respons</t>
+  </si>
+  <si>
+    <t>Kategori Kode</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>Skor %</t>
+  </si>
+  <si>
+    <t>Skor yang Diharapkan</t>
+  </si>
+  <si>
+    <t>Sangat tidak layak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21-40 </t>
+  </si>
+  <si>
+    <t>Tidak layak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41-60 </t>
+  </si>
+  <si>
+    <t>Cukup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61-80 </t>
+  </si>
+  <si>
+    <t>Layak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81-100 </t>
+  </si>
+  <si>
+    <t>Sangat layak</t>
+  </si>
+  <si>
+    <t>Rata-Rata</t>
+  </si>
+  <si>
+    <t>0-20</t>
   </si>
 </sst>
 </file>
@@ -427,9 +604,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -442,8 +619,13 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -474,6 +656,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -487,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -534,7 +722,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,22 +943,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G52" sqref="G52"/>
+      <selection pane="bottomRight" activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
@@ -778,14 +968,15 @@
     <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.5703125" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" customWidth="1"/>
-    <col min="16" max="16" width="48.42578125" customWidth="1"/>
-    <col min="17" max="17" width="52.85546875" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="23" width="18.85546875" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -841,7 +1032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="153" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>45406.60993741898</v>
       </c>
@@ -955,7 +1146,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>45406.610994456016</v>
       </c>
@@ -1340,7 +1531,7 @@
       </c>
       <c r="R10" s="11"/>
     </row>
-    <row r="11" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>45406.648065972222</v>
       </c>
@@ -1454,7 +1645,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>45406.658231990739</v>
       </c>
@@ -1511,7 +1702,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>45406.722871921302</v>
       </c>
@@ -1678,7 +1869,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>45406.765710763888</v>
       </c>
@@ -2073,7 +2264,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>45406.870665104172</v>
       </c>
@@ -2183,7 +2374,7 @@
       <c r="Q25" s="11"/>
       <c r="R25" s="11"/>
     </row>
-    <row r="26" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>45406.893882488424</v>
       </c>
@@ -2240,7 +2431,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="229.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" ht="191.25" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>45406.992285405096</v>
       </c>
@@ -2525,7 +2716,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>45407.809315439816</v>
       </c>
@@ -2582,7 +2773,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>45407.969695011576</v>
       </c>
@@ -2701,11 +2892,11 @@
         <v>120</v>
       </c>
       <c r="D36" s="14">
-        <f>CORREL(D2:D34,$O$2:$O$34)</f>
+        <f t="shared" ref="D36:N36" si="1">CORREL(D2:D34,$O$2:$O$34)</f>
         <v>0.37991897377785488</v>
       </c>
       <c r="E36" s="14">
-        <f t="shared" ref="E36:N36" si="1">CORREL(E2:E34,$O$2:$O$34)</f>
+        <f t="shared" si="1"/>
         <v>0.47178189609190446</v>
       </c>
       <c r="F36" s="14">
@@ -2913,10 +3104,17 @@
       <c r="E41" s="16" t="s">
         <v>128</v>
       </c>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="42" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="17">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="D42" s="18">
         <f>11/10*(1-P39/P38)</f>
@@ -2926,8 +3124,738 @@
         <f>IF(D42&gt;C42,"RELIABEL","TIDAK RELIABEL")</f>
         <v>RELIABEL</v>
       </c>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16" t="str">
+        <f>IF(AND(D42&gt;0.8,D42&lt;=1), "Reliabilias Sangat Tinggi", IF(AND(D42&gt;0.6,D42&lt;=0.8),"Relibilitas Tinggi",IF(AND(D42&gt;0.4,D42&lt;=0.6),"Relibilitas Sedang",IF(AND(D42&gt;0.2,D42&lt;=0.4),"Relibilitas Rendah",IF(AND(D42&gt;0,D42&lt;=0.2),"Tidak Reliabel","")))))</f>
+        <v>Relibilitas Tinggi</v>
+      </c>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="H44" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="H45" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="19"/>
+      <c r="D47" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="G47" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+    </row>
+    <row r="48" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E48" s="19">
+        <v>44</v>
+      </c>
+      <c r="F48" s="20">
+        <f>(O2/E48)*100</f>
+        <v>59.090909090909093</v>
+      </c>
+      <c r="G48" s="19" t="str">
+        <f>IF(AND(F48&gt;0,F48&lt;=20),"SANGAT TIDAK LAYAK",IF(AND(F48&gt;20,F48&lt;=40),"TIDAK LAYAK",IF(AND(F48&gt;40,F48&lt;=60),"CUKUP",IF(AND(F48&gt;60,F48&lt;=80),"LAYAK",IF(AND(F48&gt;80,F48&lt;=100),"SANGAT LAYAK","")))))</f>
+        <v>CUKUP</v>
+      </c>
+      <c r="H48" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="I48" s="19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="49" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C49" s="19"/>
+      <c r="D49" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E49" s="19">
+        <v>44</v>
+      </c>
+      <c r="F49" s="20">
+        <f t="shared" ref="F49:F50" si="4">(O3/E49)*100</f>
+        <v>63.636363636363633</v>
+      </c>
+      <c r="G49" s="19" t="str">
+        <f t="shared" ref="G49:G81" si="5">IF(AND(F49&gt;0,F49&lt;=20),"SANGAT TIDAK LAYAK",IF(AND(F49&gt;20,F49&lt;=40),"TIDAK LAYAK",IF(AND(F49&gt;40,F49&lt;=60),"CUKUP",IF(AND(F49&gt;60,F49&lt;=80),"LAYAK",IF(AND(F49&gt;80,F49&lt;=100),"SANGAT LAYAK","")))))</f>
+        <v>LAYAK</v>
+      </c>
+      <c r="H49" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="I49" s="19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C50" s="19"/>
+      <c r="D50" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="E50" s="19">
+        <v>44</v>
+      </c>
+      <c r="F50" s="20">
+        <f t="shared" si="4"/>
+        <v>63.636363636363633</v>
+      </c>
+      <c r="G50" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+      <c r="H50" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="I50" s="19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="19"/>
+      <c r="D51" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="E51" s="19">
+        <v>44</v>
+      </c>
+      <c r="F51" s="20">
+        <f>(O5/E51)*100</f>
+        <v>61.363636363636367</v>
+      </c>
+      <c r="G51" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+      <c r="H51" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="I51" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C52" s="19"/>
+      <c r="D52" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="E52" s="19">
+        <v>44</v>
+      </c>
+      <c r="F52" s="20">
+        <f t="shared" ref="F52:F80" si="6">(O6/E52)*100</f>
+        <v>61.363636363636367</v>
+      </c>
+      <c r="G52" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="I52" s="19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C53" s="19"/>
+      <c r="D53" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E53" s="19">
+        <v>44</v>
+      </c>
+      <c r="F53" s="20">
+        <f t="shared" si="6"/>
+        <v>59.090909090909093</v>
+      </c>
+      <c r="G53" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+    </row>
+    <row r="54" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="19"/>
+      <c r="D54" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E54" s="19">
+        <v>44</v>
+      </c>
+      <c r="F54" s="20">
+        <f t="shared" si="6"/>
+        <v>63.636363636363633</v>
+      </c>
+      <c r="G54" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+    </row>
+    <row r="55" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C55" s="19"/>
+      <c r="D55" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E55" s="19">
+        <v>44</v>
+      </c>
+      <c r="F55" s="20">
+        <f t="shared" si="6"/>
+        <v>52.272727272727273</v>
+      </c>
+      <c r="G55" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+    </row>
+    <row r="56" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="19"/>
+      <c r="D56" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="E56" s="19">
+        <v>44</v>
+      </c>
+      <c r="F56" s="20">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="G56" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+    </row>
+    <row r="57" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C57" s="19"/>
+      <c r="D57" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E57" s="19">
+        <v>44</v>
+      </c>
+      <c r="F57" s="20">
+        <f t="shared" si="6"/>
+        <v>61.363636363636367</v>
+      </c>
+      <c r="G57" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+    </row>
+    <row r="58" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C58" s="19"/>
+      <c r="D58" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="E58" s="19">
+        <v>44</v>
+      </c>
+      <c r="F58" s="20">
+        <f t="shared" si="6"/>
+        <v>61.363636363636367</v>
+      </c>
+      <c r="G58" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
+    </row>
+    <row r="59" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C59" s="19"/>
+      <c r="D59" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E59" s="19">
+        <v>44</v>
+      </c>
+      <c r="F59" s="20">
+        <f t="shared" si="6"/>
+        <v>54.54545454545454</v>
+      </c>
+      <c r="G59" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+    </row>
+    <row r="60" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C60" s="19"/>
+      <c r="D60" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="E60" s="19">
+        <v>44</v>
+      </c>
+      <c r="F60" s="20">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="G60" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+    </row>
+    <row r="61" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C61" s="19"/>
+      <c r="D61" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E61" s="19">
+        <v>44</v>
+      </c>
+      <c r="F61" s="20">
+        <f t="shared" si="6"/>
+        <v>59.090909090909093</v>
+      </c>
+      <c r="G61" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+    </row>
+    <row r="62" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C62" s="19"/>
+      <c r="D62" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="E62" s="19">
+        <v>44</v>
+      </c>
+      <c r="F62" s="20">
+        <f t="shared" si="6"/>
+        <v>54.54545454545454</v>
+      </c>
+      <c r="G62" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+    </row>
+    <row r="63" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C63" s="19"/>
+      <c r="D63" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E63" s="19">
+        <v>44</v>
+      </c>
+      <c r="F63" s="20">
+        <f t="shared" si="6"/>
+        <v>63.636363636363633</v>
+      </c>
+      <c r="G63" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+    </row>
+    <row r="64" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C64" s="19"/>
+      <c r="D64" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E64" s="19">
+        <v>44</v>
+      </c>
+      <c r="F64" s="20">
+        <f t="shared" si="6"/>
+        <v>45.454545454545453</v>
+      </c>
+      <c r="G64" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+    </row>
+    <row r="65" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C65" s="19"/>
+      <c r="D65" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="E65" s="19">
+        <v>44</v>
+      </c>
+      <c r="F65" s="20">
+        <f t="shared" si="6"/>
+        <v>45.454545454545453</v>
+      </c>
+      <c r="G65" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+    </row>
+    <row r="66" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C66" s="19"/>
+      <c r="D66" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="E66" s="19">
+        <v>44</v>
+      </c>
+      <c r="F66" s="20">
+        <f t="shared" si="6"/>
+        <v>63.636363636363633</v>
+      </c>
+      <c r="G66" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
+    </row>
+    <row r="67" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C67" s="19"/>
+      <c r="D67" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="E67" s="19">
+        <v>44</v>
+      </c>
+      <c r="F67" s="20">
+        <f t="shared" si="6"/>
+        <v>56.81818181818182</v>
+      </c>
+      <c r="G67" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H67" s="19"/>
+      <c r="I67" s="19"/>
+    </row>
+    <row r="68" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C68" s="19"/>
+      <c r="D68" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="E68" s="19">
+        <v>44</v>
+      </c>
+      <c r="F68" s="20">
+        <f t="shared" si="6"/>
+        <v>43.18181818181818</v>
+      </c>
+      <c r="G68" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H68" s="19"/>
+      <c r="I68" s="19"/>
+    </row>
+    <row r="69" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C69" s="19"/>
+      <c r="D69" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="E69" s="19">
+        <v>44</v>
+      </c>
+      <c r="F69" s="20">
+        <f t="shared" si="6"/>
+        <v>63.636363636363633</v>
+      </c>
+      <c r="G69" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+      <c r="H69" s="19"/>
+      <c r="I69" s="19"/>
+    </row>
+    <row r="70" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C70" s="19"/>
+      <c r="D70" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E70" s="19">
+        <v>44</v>
+      </c>
+      <c r="F70" s="20">
+        <f t="shared" si="6"/>
+        <v>63.636363636363633</v>
+      </c>
+      <c r="G70" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+      <c r="H70" s="19"/>
+      <c r="I70" s="19"/>
+    </row>
+    <row r="71" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C71" s="19"/>
+      <c r="D71" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E71" s="19">
+        <v>44</v>
+      </c>
+      <c r="F71" s="20">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="G71" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H71" s="19"/>
+      <c r="I71" s="19"/>
+    </row>
+    <row r="72" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C72" s="19"/>
+      <c r="D72" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E72" s="19">
+        <v>44</v>
+      </c>
+      <c r="F72" s="20">
+        <f t="shared" si="6"/>
+        <v>47.727272727272727</v>
+      </c>
+      <c r="G72" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H72" s="19"/>
+      <c r="I72" s="19"/>
+    </row>
+    <row r="73" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C73" s="19"/>
+      <c r="D73" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="E73" s="19">
+        <v>44</v>
+      </c>
+      <c r="F73" s="20">
+        <f t="shared" si="6"/>
+        <v>63.636363636363633</v>
+      </c>
+      <c r="G73" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+      <c r="H73" s="19"/>
+      <c r="I73" s="19"/>
+    </row>
+    <row r="74" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C74" s="19"/>
+      <c r="D74" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="E74" s="19">
+        <v>44</v>
+      </c>
+      <c r="F74" s="20">
+        <f t="shared" si="6"/>
+        <v>54.54545454545454</v>
+      </c>
+      <c r="G74" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H74" s="19"/>
+      <c r="I74" s="19"/>
+    </row>
+    <row r="75" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C75" s="19"/>
+      <c r="D75" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="E75" s="19">
+        <v>44</v>
+      </c>
+      <c r="F75" s="20">
+        <f t="shared" si="6"/>
+        <v>63.636363636363633</v>
+      </c>
+      <c r="G75" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+      <c r="H75" s="19"/>
+      <c r="I75" s="19"/>
+    </row>
+    <row r="76" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C76" s="19"/>
+      <c r="D76" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="E76" s="19">
+        <v>44</v>
+      </c>
+      <c r="F76" s="20">
+        <f t="shared" si="6"/>
+        <v>59.090909090909093</v>
+      </c>
+      <c r="G76" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H76" s="19"/>
+      <c r="I76" s="19"/>
+    </row>
+    <row r="77" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C77" s="19"/>
+      <c r="D77" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="E77" s="19">
+        <v>44</v>
+      </c>
+      <c r="F77" s="20">
+        <f t="shared" si="6"/>
+        <v>59.090909090909093</v>
+      </c>
+      <c r="G77" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H77" s="19"/>
+      <c r="I77" s="19"/>
+    </row>
+    <row r="78" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C78" s="19"/>
+      <c r="D78" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="E78" s="19">
+        <v>44</v>
+      </c>
+      <c r="F78" s="20">
+        <f t="shared" si="6"/>
+        <v>52.272727272727273</v>
+      </c>
+      <c r="G78" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H78" s="19"/>
+      <c r="I78" s="19"/>
+    </row>
+    <row r="79" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C79" s="19"/>
+      <c r="D79" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="E79" s="19">
+        <v>44</v>
+      </c>
+      <c r="F79" s="20">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="G79" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H79" s="19"/>
+      <c r="I79" s="19"/>
+    </row>
+    <row r="80" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C80" s="19"/>
+      <c r="D80" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="E80" s="19">
+        <v>44</v>
+      </c>
+      <c r="F80" s="20">
+        <f t="shared" si="6"/>
+        <v>63.636363636363633</v>
+      </c>
+      <c r="G80" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
+    </row>
+    <row r="81" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C81" s="19"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="F81" s="20">
+        <f>AVERAGE(F48:F80)</f>
+        <v>57.093663911845738</v>
+      </c>
+      <c r="G81" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>CUKUP</v>
+      </c>
+      <c r="H81" s="19"/>
+      <c r="I81" s="19"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>